<commit_message>
Update release candidate: V 0.9Build7 - add Persist user settings - add User settings for number of aircrafts supported - add Logging debug support - add Readme/Guide for Script Language - add Optional scripting for accel and turnrates, new Msl Alt mode - update Throttle the LT sender to avoid excess CPU usage - update Use script and model for IFR flight creation - update Refactor aircraft, sim parts, review/update comments - update Some misleading names - update Use Bluebird CSL supported aircrafts and operators for IFR flights - update Provide callsign, tail registration and airborne tag to LT - fix Change to ground speed (GS) naming to match AITRAFFIC format
</commit_message>
<xml_diff>
--- a/Doc/TrackCalc.xlsx
+++ b/Doc/TrackCalc.xlsx
@@ -141,7 +141,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -395,16 +395,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -715,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,55 +861,55 @@
         <v>13</v>
       </c>
       <c r="C6" s="10">
-        <f>C$5/(20*PI()*$C$52)</f>
+        <f t="shared" ref="C6:O6" si="1">C$5/(20*PI()*$C$52)</f>
         <v>0.31830988618379069</v>
       </c>
       <c r="D6" s="10">
-        <f>D$5/(20*PI()*$C$52)</f>
+        <f t="shared" si="1"/>
         <v>0.37136153388108917</v>
       </c>
       <c r="E6" s="10">
-        <f>E$5/(20*PI()*$C$52)</f>
+        <f t="shared" si="1"/>
         <v>0.42441318157838759</v>
       </c>
       <c r="F6" s="10">
-        <f>F$5/(20*PI()*$C$52)</f>
+        <f t="shared" si="1"/>
         <v>0.47746482927568606</v>
       </c>
       <c r="G6" s="10">
-        <f>G$5/(20*PI()*$C$52)</f>
+        <f t="shared" si="1"/>
         <v>0.53051647697298454</v>
       </c>
       <c r="H6" s="10">
-        <f>H$5/(20*PI()*$C$52)</f>
+        <f t="shared" si="1"/>
         <v>0.58356812467028296</v>
       </c>
       <c r="I6" s="10">
-        <f>I$5/(20*PI()*$C$52)</f>
+        <f t="shared" si="1"/>
         <v>0.63661977236758138</v>
       </c>
       <c r="J6" s="10">
-        <f>J$5/(20*PI()*$C$52)</f>
+        <f t="shared" si="1"/>
         <v>0.68967142006487991</v>
       </c>
       <c r="K6" s="10">
-        <f>K$5/(20*PI()*$C$52)</f>
+        <f t="shared" si="1"/>
         <v>0.74272306776217834</v>
       </c>
       <c r="L6" s="10">
-        <f>L$5/(20*PI()*$C$52)</f>
+        <f t="shared" si="1"/>
         <v>0.79577471545947676</v>
       </c>
       <c r="M6" s="10">
-        <f>M$5/(20*PI()*$C$52)</f>
+        <f t="shared" si="1"/>
         <v>0.84882636315677518</v>
       </c>
       <c r="N6" s="10">
-        <f>N$5/(20*PI()*$C$52)</f>
+        <f t="shared" si="1"/>
         <v>0.90187801085407371</v>
       </c>
       <c r="O6" s="17">
-        <f>O$5/(20*PI()*$C$52)</f>
+        <f t="shared" si="1"/>
         <v>0.95492965855137213</v>
       </c>
     </row>
@@ -921,55 +921,55 @@
         <v>13</v>
       </c>
       <c r="C7" s="20">
-        <f>C$5/3600*($C$4/$C$52)</f>
+        <f t="shared" ref="C7:O7" si="2">C$5/3600*($C$4/$C$52)</f>
         <v>0.5</v>
       </c>
       <c r="D7" s="20">
-        <f>D$5/3600*($C$4/$C$52)</f>
+        <f t="shared" si="2"/>
         <v>0.58333333333333337</v>
       </c>
       <c r="E7" s="20">
-        <f>E$5/3600*($C$4/$C$52)</f>
+        <f t="shared" si="2"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="F7" s="20">
-        <f>F$5/3600*($C$4/$C$52)</f>
+        <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
       <c r="G7" s="20">
-        <f>G$5/3600*($C$4/$C$52)</f>
+        <f t="shared" si="2"/>
         <v>0.83333333333333326</v>
       </c>
       <c r="H7" s="20">
-        <f>H$5/3600*($C$4/$C$52)</f>
+        <f t="shared" si="2"/>
         <v>0.91666666666666663</v>
       </c>
       <c r="I7" s="20">
-        <f>I$5/3600*($C$4/$C$52)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J7" s="20">
-        <f>J$5/3600*($C$4/$C$52)</f>
+        <f t="shared" si="2"/>
         <v>1.0833333333333333</v>
       </c>
       <c r="K7" s="20">
-        <f>K$5/3600*($C$4/$C$52)</f>
+        <f t="shared" si="2"/>
         <v>1.1666666666666667</v>
       </c>
       <c r="L7" s="20">
-        <f>L$5/3600*($C$4/$C$52)</f>
+        <f t="shared" si="2"/>
         <v>1.25</v>
       </c>
       <c r="M7" s="20">
-        <f>M$5/3600*($C$4/$C$52)</f>
+        <f t="shared" si="2"/>
         <v>1.3333333333333335</v>
       </c>
       <c r="N7" s="20">
-        <f>N$5/3600*($C$4/$C$52)</f>
+        <f t="shared" si="2"/>
         <v>1.4166666666666665</v>
       </c>
       <c r="O7" s="21">
-        <f>O$5/3600*($C$4/$C$52)</f>
+        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1033,47 +1033,47 @@
         <v>30</v>
       </c>
       <c r="E11" s="9">
-        <f t="shared" ref="E11:O11" si="1">D11+$P11</f>
+        <f t="shared" ref="E11:O11" si="3">D11+$P11</f>
         <v>60</v>
       </c>
       <c r="F11" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
       <c r="G11" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="H11" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="I11" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="J11" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>210</v>
       </c>
       <c r="K11" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>240</v>
       </c>
       <c r="L11" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>270</v>
       </c>
       <c r="M11" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>300</v>
       </c>
       <c r="N11" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>330</v>
       </c>
       <c r="O11" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>360</v>
       </c>
       <c r="P11" s="40">
@@ -1112,55 +1112,55 @@
         <v>13</v>
       </c>
       <c r="C13" s="20">
-        <f>$C$10/3600*(C11/$C$52)</f>
+        <f t="shared" ref="C13:O13" si="4">$C$10/3600*(C11/$C$52)</f>
         <v>0</v>
       </c>
       <c r="D13" s="20">
-        <f>$C$10/3600*(D11/$C$52)</f>
+        <f t="shared" si="4"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="E13" s="20">
-        <f>$C$10/3600*(E11/$C$52)</f>
+        <f t="shared" si="4"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="F13" s="20">
-        <f>$C$10/3600*(F11/$C$52)</f>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="G13" s="20">
-        <f>$C$10/3600*(G11/$C$52)</f>
+        <f t="shared" si="4"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="H13" s="20">
-        <f>$C$10/3600*(H11/$C$52)</f>
+        <f t="shared" si="4"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="I13" s="20">
-        <f>$C$10/3600*(I11/$C$52)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J13" s="20">
-        <f>$C$10/3600*(J11/$C$52)</f>
+        <f t="shared" si="4"/>
         <v>1.1666666666666667</v>
       </c>
       <c r="K13" s="20">
-        <f>$C$10/3600*(K11/$C$52)</f>
+        <f t="shared" si="4"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="L13" s="20">
-        <f>$C$10/3600*(L11/$C$52)</f>
+        <f t="shared" si="4"/>
         <v>1.5</v>
       </c>
       <c r="M13" s="20">
-        <f>$C$10/3600*(M11/$C$52)</f>
+        <f t="shared" si="4"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="N13" s="20">
-        <f>$C$10/3600*(N11/$C$52)</f>
+        <f t="shared" si="4"/>
         <v>1.8333333333333333</v>
       </c>
       <c r="O13" s="21">
-        <f>$C$10/3600*(O11/$C$52)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -1224,47 +1224,47 @@
         <v>2</v>
       </c>
       <c r="E18" s="9">
-        <f t="shared" ref="E18:O18" si="2">D18+$P18</f>
+        <f t="shared" ref="E18:O18" si="5">D18+$P18</f>
         <v>3</v>
       </c>
       <c r="F18" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G18" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="H18" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="I18" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="J18" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="K18" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="L18" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="M18" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="N18" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="O18" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="P18" s="40">
@@ -1279,55 +1279,55 @@
         <v>16</v>
       </c>
       <c r="C19" s="26">
-        <f>C18/($C$17/3600)</f>
+        <f t="shared" ref="C19:O19" si="6">C18/($C$17/3600)</f>
         <v>60</v>
       </c>
       <c r="D19" s="26">
-        <f>D18/($C$17/3600)</f>
+        <f t="shared" si="6"/>
         <v>120</v>
       </c>
       <c r="E19" s="26">
-        <f>E18/($C$17/3600)</f>
+        <f t="shared" si="6"/>
         <v>180</v>
       </c>
       <c r="F19" s="26">
-        <f>F18/($C$17/3600)</f>
+        <f t="shared" si="6"/>
         <v>240</v>
       </c>
       <c r="G19" s="26">
-        <f>G18/($C$17/3600)</f>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="H19" s="26">
-        <f>H18/($C$17/3600)</f>
+        <f t="shared" si="6"/>
         <v>360</v>
       </c>
       <c r="I19" s="26">
-        <f>I18/($C$17/3600)</f>
+        <f t="shared" si="6"/>
         <v>420</v>
       </c>
       <c r="J19" s="26">
-        <f>J18/($C$17/3600)</f>
+        <f t="shared" si="6"/>
         <v>480</v>
       </c>
       <c r="K19" s="26">
-        <f>K18/($C$17/3600)</f>
+        <f t="shared" si="6"/>
         <v>540</v>
       </c>
       <c r="L19" s="26">
-        <f>L18/($C$17/3600)</f>
+        <f t="shared" si="6"/>
         <v>600</v>
       </c>
       <c r="M19" s="26">
-        <f>M18/($C$17/3600)</f>
+        <f t="shared" si="6"/>
         <v>660</v>
       </c>
       <c r="N19" s="26">
-        <f>N18/($C$17/3600)</f>
+        <f t="shared" si="6"/>
         <v>720</v>
       </c>
       <c r="O19" s="27">
-        <f>O18/($C$17/3600)</f>
+        <f t="shared" si="6"/>
         <v>780</v>
       </c>
     </row>
@@ -1337,55 +1337,55 @@
         <v>18</v>
       </c>
       <c r="C20" s="28">
-        <f>C19/60</f>
+        <f t="shared" ref="C20:O20" si="7">C19/60</f>
         <v>1</v>
       </c>
       <c r="D20" s="28">
-        <f>D19/60</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="E20" s="28">
-        <f>E19/60</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="F20" s="28">
-        <f>F19/60</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="G20" s="28">
-        <f>G19/60</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="H20" s="28">
-        <f>H19/60</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="I20" s="28">
-        <f>I19/60</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="J20" s="28">
-        <f>J19/60</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="K20" s="28">
-        <f>K19/60</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="L20" s="28">
-        <f>L19/60</f>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="M20" s="28">
-        <f>M19/60</f>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="N20" s="28">
-        <f>N19/60</f>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="O20" s="29">
-        <f>O19/60</f>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
     </row>
@@ -1449,47 +1449,47 @@
         <v>70</v>
       </c>
       <c r="E24" s="9">
-        <f t="shared" ref="E24:O24" si="3">D24++$P24</f>
+        <f t="shared" ref="E24:O24" si="8">D24++$P24</f>
         <v>80</v>
       </c>
       <c r="F24" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>90</v>
       </c>
       <c r="G24" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="H24" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>110</v>
       </c>
       <c r="I24" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>120</v>
       </c>
       <c r="J24" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>130</v>
       </c>
       <c r="K24" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>140</v>
       </c>
       <c r="L24" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>150</v>
       </c>
       <c r="M24" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>160</v>
       </c>
       <c r="N24" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>170</v>
       </c>
       <c r="O24" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>180</v>
       </c>
       <c r="P24" s="40">
@@ -1508,51 +1508,51 @@
         <v>600</v>
       </c>
       <c r="D25" s="30">
-        <f t="shared" ref="D25:O25" si="4">$C23/(D24/3600)</f>
+        <f t="shared" ref="D25:O25" si="9">$C23/(D24/3600)</f>
         <v>514.28571428571422</v>
       </c>
       <c r="E25" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>450</v>
       </c>
       <c r="F25" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>400</v>
       </c>
       <c r="G25" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>360</v>
       </c>
       <c r="H25" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>327.27272727272731</v>
       </c>
       <c r="I25" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>300</v>
       </c>
       <c r="J25" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>276.92307692307696</v>
       </c>
       <c r="K25" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>257.14285714285711</v>
       </c>
       <c r="L25" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>240</v>
       </c>
       <c r="M25" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>225</v>
       </c>
       <c r="N25" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>211.76470588235296</v>
       </c>
       <c r="O25" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>200</v>
       </c>
     </row>
@@ -1566,51 +1566,51 @@
         <v>10</v>
       </c>
       <c r="D26" s="28">
-        <f t="shared" ref="D26:O26" si="5">D25/60</f>
+        <f t="shared" ref="D26:O26" si="10">D25/60</f>
         <v>8.5714285714285712</v>
       </c>
       <c r="E26" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>7.5</v>
       </c>
       <c r="F26" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>6.666666666666667</v>
       </c>
       <c r="G26" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="H26" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>5.454545454545455</v>
       </c>
       <c r="I26" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="J26" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>4.6153846153846159</v>
       </c>
       <c r="K26" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>4.2857142857142856</v>
       </c>
       <c r="L26" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="M26" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>3.75</v>
       </c>
       <c r="N26" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>3.5294117647058827</v>
       </c>
       <c r="O26" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>3.3333333333333335</v>
       </c>
     </row>
@@ -1674,47 +1674,47 @@
         <v>400</v>
       </c>
       <c r="E31" s="9">
-        <f t="shared" ref="E31:O31" si="6">D31+$P31</f>
+        <f t="shared" ref="E31:O31" si="11">D31+$P31</f>
         <v>500</v>
       </c>
       <c r="F31" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>600</v>
       </c>
       <c r="G31" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>700</v>
       </c>
       <c r="H31" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>800</v>
       </c>
       <c r="I31" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>900</v>
       </c>
       <c r="J31" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1000</v>
       </c>
       <c r="K31" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1100</v>
       </c>
       <c r="L31" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1200</v>
       </c>
       <c r="M31" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1300</v>
       </c>
       <c r="N31" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1400</v>
       </c>
       <c r="O31" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1500</v>
       </c>
       <c r="P31" s="40">
@@ -1733,51 +1733,51 @@
         <v>400</v>
       </c>
       <c r="D32" s="30">
-        <f t="shared" ref="D32:O32" si="7">$C30/(D31/60)</f>
+        <f t="shared" ref="D32:O32" si="12">$C30/(D31/60)</f>
         <v>300</v>
       </c>
       <c r="E32" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>239.99999999999997</v>
       </c>
       <c r="F32" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>200</v>
       </c>
       <c r="G32" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>171.42857142857144</v>
       </c>
       <c r="H32" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>150</v>
       </c>
       <c r="I32" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>133.33333333333334</v>
       </c>
       <c r="J32" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>119.99999999999999</v>
       </c>
       <c r="K32" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>109.09090909090909</v>
       </c>
       <c r="L32" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>100</v>
       </c>
       <c r="M32" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>92.307692307692307</v>
       </c>
       <c r="N32" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>85.714285714285722</v>
       </c>
       <c r="O32" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>80</v>
       </c>
     </row>
@@ -1791,51 +1791,51 @@
         <v>6.666666666666667</v>
       </c>
       <c r="D33" s="28">
-        <f t="shared" ref="D33:O33" si="8">D32/60</f>
+        <f t="shared" ref="D33:O33" si="13">D32/60</f>
         <v>5</v>
       </c>
       <c r="E33" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>3.9999999999999996</v>
       </c>
       <c r="F33" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="G33" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>2.8571428571428572</v>
       </c>
       <c r="H33" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>2.5</v>
       </c>
       <c r="I33" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>2.2222222222222223</v>
       </c>
       <c r="J33" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1.9999999999999998</v>
       </c>
       <c r="K33" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1.8181818181818181</v>
       </c>
       <c r="L33" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="M33" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1.5384615384615385</v>
       </c>
       <c r="N33" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="O33" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1.3333333333333333</v>
       </c>
     </row>
@@ -1899,47 +1899,47 @@
         <v>200</v>
       </c>
       <c r="E37" s="9">
-        <f t="shared" ref="E37:O37" si="9">D37+$P37</f>
+        <f t="shared" ref="E37:O37" si="14">D37+$P37</f>
         <v>400</v>
       </c>
       <c r="F37" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>600</v>
       </c>
       <c r="G37" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>800</v>
       </c>
       <c r="H37" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>1000</v>
       </c>
       <c r="I37" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>1200</v>
       </c>
       <c r="J37" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>1400</v>
       </c>
       <c r="K37" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>1600</v>
       </c>
       <c r="L37" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>1800</v>
       </c>
       <c r="M37" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>2000</v>
       </c>
       <c r="N37" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>2200</v>
       </c>
       <c r="O37" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>2400</v>
       </c>
       <c r="P37" s="40">
@@ -1958,51 +1958,51 @@
         <v>0</v>
       </c>
       <c r="D38" s="30">
-        <f t="shared" ref="D38:O38" si="10">D37/($C36/60)</f>
+        <f t="shared" ref="D38:O38" si="15">D37/($C36/60)</f>
         <v>12</v>
       </c>
       <c r="E38" s="30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>24</v>
       </c>
       <c r="F38" s="30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>36</v>
       </c>
       <c r="G38" s="30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>48</v>
       </c>
       <c r="H38" s="30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>59.999999999999993</v>
       </c>
       <c r="I38" s="30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>72</v>
       </c>
       <c r="J38" s="30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>84</v>
       </c>
       <c r="K38" s="30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>96</v>
       </c>
       <c r="L38" s="30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>107.99999999999999</v>
       </c>
       <c r="M38" s="30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>119.99999999999999</v>
       </c>
       <c r="N38" s="30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>132</v>
       </c>
       <c r="O38" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>144</v>
       </c>
     </row>
@@ -2016,51 +2016,51 @@
         <v>0</v>
       </c>
       <c r="D39" s="28">
-        <f t="shared" ref="D39" si="11">D38/60</f>
+        <f t="shared" ref="D39" si="16">D38/60</f>
         <v>0.2</v>
       </c>
       <c r="E39" s="28">
-        <f t="shared" ref="E39" si="12">E38/60</f>
+        <f t="shared" ref="E39" si="17">E38/60</f>
         <v>0.4</v>
       </c>
       <c r="F39" s="28">
-        <f t="shared" ref="F39" si="13">F38/60</f>
+        <f t="shared" ref="F39" si="18">F38/60</f>
         <v>0.6</v>
       </c>
       <c r="G39" s="28">
-        <f t="shared" ref="G39" si="14">G38/60</f>
+        <f t="shared" ref="G39" si="19">G38/60</f>
         <v>0.8</v>
       </c>
       <c r="H39" s="28">
-        <f t="shared" ref="H39" si="15">H38/60</f>
+        <f t="shared" ref="H39" si="20">H38/60</f>
         <v>0.99999999999999989</v>
       </c>
       <c r="I39" s="28">
-        <f t="shared" ref="I39" si="16">I38/60</f>
+        <f t="shared" ref="I39" si="21">I38/60</f>
         <v>1.2</v>
       </c>
       <c r="J39" s="28">
-        <f t="shared" ref="J39" si="17">J38/60</f>
+        <f t="shared" ref="J39" si="22">J38/60</f>
         <v>1.4</v>
       </c>
       <c r="K39" s="28">
-        <f t="shared" ref="K39" si="18">K38/60</f>
+        <f t="shared" ref="K39" si="23">K38/60</f>
         <v>1.6</v>
       </c>
       <c r="L39" s="28">
-        <f t="shared" ref="L39" si="19">L38/60</f>
+        <f t="shared" ref="L39" si="24">L38/60</f>
         <v>1.7999999999999998</v>
       </c>
       <c r="M39" s="28">
-        <f t="shared" ref="M39" si="20">M38/60</f>
+        <f t="shared" ref="M39" si="25">M38/60</f>
         <v>1.9999999999999998</v>
       </c>
       <c r="N39" s="28">
-        <f t="shared" ref="N39" si="21">N38/60</f>
+        <f t="shared" ref="N39" si="26">N38/60</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="O39" s="29">
-        <f t="shared" ref="O39" si="22">O38/60</f>
+        <f t="shared" ref="O39" si="27">O38/60</f>
         <v>2.4</v>
       </c>
     </row>
@@ -2117,55 +2117,55 @@
         <v>6</v>
       </c>
       <c r="C43" s="8">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="D43" s="9">
         <f>C43+$P43</f>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="E43" s="9">
-        <f t="shared" ref="E43:O43" si="23">D43+$P43</f>
-        <v>80</v>
+        <f t="shared" ref="E43:O43" si="28">D43+$P43</f>
+        <v>120</v>
       </c>
       <c r="F43" s="9">
-        <f t="shared" si="23"/>
-        <v>90</v>
+        <f t="shared" si="28"/>
+        <v>130</v>
       </c>
       <c r="G43" s="9">
-        <f t="shared" si="23"/>
-        <v>100</v>
+        <f t="shared" si="28"/>
+        <v>140</v>
       </c>
       <c r="H43" s="9">
-        <f t="shared" si="23"/>
-        <v>110</v>
+        <f t="shared" si="28"/>
+        <v>150</v>
       </c>
       <c r="I43" s="9">
-        <f t="shared" si="23"/>
-        <v>120</v>
+        <f t="shared" si="28"/>
+        <v>160</v>
       </c>
       <c r="J43" s="9">
-        <f t="shared" si="23"/>
-        <v>130</v>
+        <f t="shared" si="28"/>
+        <v>170</v>
       </c>
       <c r="K43" s="9">
-        <f t="shared" si="23"/>
-        <v>140</v>
+        <f t="shared" si="28"/>
+        <v>180</v>
       </c>
       <c r="L43" s="9">
-        <f t="shared" si="23"/>
-        <v>150</v>
+        <f t="shared" si="28"/>
+        <v>190</v>
       </c>
       <c r="M43" s="9">
-        <f t="shared" si="23"/>
-        <v>160</v>
+        <f t="shared" si="28"/>
+        <v>200</v>
       </c>
       <c r="N43" s="9">
-        <f t="shared" si="23"/>
-        <v>170</v>
+        <f t="shared" si="28"/>
+        <v>210</v>
       </c>
       <c r="O43" s="16">
-        <f t="shared" si="23"/>
-        <v>180</v>
+        <f t="shared" si="28"/>
+        <v>220</v>
       </c>
       <c r="P43" s="40">
         <v>10</v>
@@ -2180,55 +2180,55 @@
       </c>
       <c r="C44" s="32">
         <f>(C43-$C42)/$C$51</f>
-        <v>20</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="D44" s="32">
-        <f t="shared" ref="D44:O44" si="24">(D43-$C42)/$C$51</f>
-        <v>23.333333333333332</v>
+        <f t="shared" ref="D44:O44" si="29">(D43-$C42)/$C$51</f>
+        <v>36.666666666666664</v>
       </c>
       <c r="E44" s="32">
-        <f t="shared" si="24"/>
-        <v>26.666666666666668</v>
+        <f t="shared" si="29"/>
+        <v>40</v>
       </c>
       <c r="F44" s="32">
-        <f t="shared" si="24"/>
-        <v>30</v>
+        <f t="shared" si="29"/>
+        <v>43.333333333333336</v>
       </c>
       <c r="G44" s="32">
-        <f t="shared" si="24"/>
-        <v>33.333333333333336</v>
+        <f t="shared" si="29"/>
+        <v>46.666666666666664</v>
       </c>
       <c r="H44" s="32">
-        <f t="shared" si="24"/>
-        <v>36.666666666666664</v>
+        <f t="shared" si="29"/>
+        <v>50</v>
       </c>
       <c r="I44" s="32">
-        <f t="shared" si="24"/>
-        <v>40</v>
+        <f t="shared" si="29"/>
+        <v>53.333333333333336</v>
       </c>
       <c r="J44" s="32">
-        <f t="shared" si="24"/>
-        <v>43.333333333333336</v>
+        <f t="shared" si="29"/>
+        <v>56.666666666666664</v>
       </c>
       <c r="K44" s="32">
-        <f t="shared" si="24"/>
-        <v>46.666666666666664</v>
+        <f t="shared" si="29"/>
+        <v>60</v>
       </c>
       <c r="L44" s="32">
-        <f t="shared" si="24"/>
-        <v>50</v>
+        <f t="shared" si="29"/>
+        <v>63.333333333333336</v>
       </c>
       <c r="M44" s="32">
-        <f t="shared" si="24"/>
-        <v>53.333333333333336</v>
+        <f t="shared" si="29"/>
+        <v>66.666666666666671</v>
       </c>
       <c r="N44" s="32">
-        <f t="shared" si="24"/>
-        <v>56.666666666666664</v>
+        <f t="shared" si="29"/>
+        <v>70</v>
       </c>
       <c r="O44" s="33">
-        <f t="shared" si="24"/>
-        <v>60</v>
+        <f t="shared" si="29"/>
+        <v>73.333333333333329</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -2238,55 +2238,55 @@
       </c>
       <c r="C45" s="34">
         <f>C44/60</f>
-        <v>0.33333333333333331</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="D45" s="34">
-        <f t="shared" ref="D45" si="25">D44/60</f>
-        <v>0.3888888888888889</v>
+        <f t="shared" ref="D45" si="30">D44/60</f>
+        <v>0.61111111111111105</v>
       </c>
       <c r="E45" s="34">
-        <f t="shared" ref="E45" si="26">E44/60</f>
-        <v>0.44444444444444448</v>
+        <f t="shared" ref="E45" si="31">E44/60</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F45" s="34">
-        <f t="shared" ref="F45" si="27">F44/60</f>
-        <v>0.5</v>
+        <f t="shared" ref="F45" si="32">F44/60</f>
+        <v>0.72222222222222221</v>
       </c>
       <c r="G45" s="34">
-        <f t="shared" ref="G45" si="28">G44/60</f>
-        <v>0.55555555555555558</v>
+        <f t="shared" ref="G45" si="33">G44/60</f>
+        <v>0.77777777777777779</v>
       </c>
       <c r="H45" s="34">
-        <f t="shared" ref="H45" si="29">H44/60</f>
-        <v>0.61111111111111105</v>
+        <f t="shared" ref="H45" si="34">H44/60</f>
+        <v>0.83333333333333337</v>
       </c>
       <c r="I45" s="34">
-        <f t="shared" ref="I45" si="30">I44/60</f>
-        <v>0.66666666666666663</v>
+        <f t="shared" ref="I45" si="35">I44/60</f>
+        <v>0.88888888888888895</v>
       </c>
       <c r="J45" s="34">
-        <f t="shared" ref="J45" si="31">J44/60</f>
-        <v>0.72222222222222221</v>
+        <f t="shared" ref="J45" si="36">J44/60</f>
+        <v>0.94444444444444442</v>
       </c>
       <c r="K45" s="34">
-        <f t="shared" ref="K45" si="32">K44/60</f>
-        <v>0.77777777777777779</v>
+        <f t="shared" ref="K45" si="37">K44/60</f>
+        <v>1</v>
       </c>
       <c r="L45" s="34">
-        <f t="shared" ref="L45" si="33">L44/60</f>
-        <v>0.83333333333333337</v>
+        <f t="shared" ref="L45" si="38">L44/60</f>
+        <v>1.0555555555555556</v>
       </c>
       <c r="M45" s="34">
-        <f t="shared" ref="M45" si="34">M44/60</f>
-        <v>0.88888888888888895</v>
+        <f t="shared" ref="M45" si="39">M44/60</f>
+        <v>1.1111111111111112</v>
       </c>
       <c r="N45" s="34">
-        <f t="shared" ref="N45" si="35">N44/60</f>
-        <v>0.94444444444444442</v>
+        <f t="shared" ref="N45" si="40">N44/60</f>
+        <v>1.1666666666666667</v>
       </c>
       <c r="O45" s="35">
-        <f t="shared" ref="O45" si="36">O44/60</f>
-        <v>1</v>
+        <f t="shared" ref="O45" si="41">O44/60</f>
+        <v>1.2222222222222221</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2298,55 +2298,55 @@
       </c>
       <c r="C46" s="36">
         <f>(C43*C43-$C42*$C42)/(2*$C$51*3600)</f>
-        <v>0.16666666666666666</v>
+        <v>0.46296296296296297</v>
       </c>
       <c r="D46" s="36">
-        <f t="shared" ref="D46:O46" si="37">(D43*D43-$C42*$C42)/(2*$C$51*3600)</f>
-        <v>0.22685185185185186</v>
+        <f t="shared" ref="D46:O46" si="42">(D43*D43-$C42*$C42)/(2*$C$51*3600)</f>
+        <v>0.56018518518518523</v>
       </c>
       <c r="E46" s="36">
-        <f t="shared" si="37"/>
-        <v>0.29629629629629628</v>
+        <f t="shared" si="42"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F46" s="36">
-        <f t="shared" si="37"/>
-        <v>0.375</v>
+        <f t="shared" si="42"/>
+        <v>0.78240740740740744</v>
       </c>
       <c r="G46" s="36">
-        <f t="shared" si="37"/>
-        <v>0.46296296296296297</v>
+        <f t="shared" si="42"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="H46" s="36">
-        <f t="shared" si="37"/>
-        <v>0.56018518518518523</v>
+        <f t="shared" si="42"/>
+        <v>1.0416666666666667</v>
       </c>
       <c r="I46" s="36">
-        <f t="shared" si="37"/>
-        <v>0.66666666666666663</v>
+        <f t="shared" si="42"/>
+        <v>1.1851851851851851</v>
       </c>
       <c r="J46" s="36">
-        <f t="shared" si="37"/>
-        <v>0.78240740740740744</v>
+        <f t="shared" si="42"/>
+        <v>1.337962962962963</v>
       </c>
       <c r="K46" s="36">
-        <f t="shared" si="37"/>
-        <v>0.90740740740740744</v>
+        <f t="shared" si="42"/>
+        <v>1.5</v>
       </c>
       <c r="L46" s="36">
-        <f t="shared" si="37"/>
-        <v>1.0416666666666667</v>
+        <f t="shared" si="42"/>
+        <v>1.6712962962962963</v>
       </c>
       <c r="M46" s="36">
-        <f t="shared" si="37"/>
-        <v>1.1851851851851851</v>
+        <f t="shared" si="42"/>
+        <v>1.8518518518518519</v>
       </c>
       <c r="N46" s="36">
-        <f t="shared" si="37"/>
-        <v>1.337962962962963</v>
+        <f t="shared" si="42"/>
+        <v>2.0416666666666665</v>
       </c>
       <c r="O46" s="37">
-        <f t="shared" si="37"/>
-        <v>1.5</v>
+        <f t="shared" si="42"/>
+        <v>2.2407407407407409</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>